<commit_message>
create histogram and pareto chart
</commit_message>
<xml_diff>
--- a/Secondo progetto/Exercise1.xlsx
+++ b/Secondo progetto/Exercise1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enrico\Desktop\Lavoro\Corso Methods and tools (Sacile)\CorsoControlloQualità\Esercizi 2018_2019\EserciziStudenti\Esercizio1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio\Documents\GitHub\method_proect_one\Secondo progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E29E35-7CA1-41ED-9621-F72F7ED91F0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12030"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -167,18 +168,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -461,14 +462,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C9"/>
+      <selection activeCell="B5" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
@@ -479,78 +485,78 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="8">
         <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="6">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="6">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="6">
         <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="8">
         <v>137</v>
       </c>
     </row>
@@ -560,5 +566,6 @@
     <mergeCell ref="A6:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
start to create dataset for c chart
</commit_message>
<xml_diff>
--- a/Secondo progetto/Exercise1.xlsx
+++ b/Secondo progetto/Exercise1.xlsx
@@ -8,24 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonio\Documents\GitHub\method_proect_one\Secondo progetto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E29E35-7CA1-41ED-9621-F72F7ED91F0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7EFCA1-DBFB-43E4-85C3-20541925B0BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>Fault</t>
   </si>
@@ -49,6 +54,12 @@
   </si>
   <si>
     <t>Evening shift</t>
+  </si>
+  <si>
+    <t>Total Evening</t>
+  </si>
+  <si>
+    <t>Total morning</t>
   </si>
 </sst>
 </file>
@@ -463,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B2:B5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,9 +485,10 @@
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -484,7 +496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
@@ -495,7 +507,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="5" t="s">
         <v>4</v>
@@ -503,8 +515,15 @@
       <c r="C3" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <f>SUM(C2:C5)</f>
+        <v>312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="5" t="s">
         <v>5</v>
@@ -513,7 +532,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="7" t="s">
         <v>6</v>
@@ -522,7 +541,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
@@ -533,7 +552,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="5" t="s">
         <v>4</v>
@@ -541,8 +560,15 @@
       <c r="C7" s="6">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <f>SUM(C6:C9)</f>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="5" t="s">
         <v>5</v>
@@ -551,7 +577,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="7" t="s">
         <v>6</v>

</xml_diff>